<commit_message>
PAE - MultiHiper - inclusão da nota do simulado sem nome
</commit_message>
<xml_diff>
--- a/3-PAE/SCC0611-MultHiper/Notas-simulado.xlsx
+++ b/3-PAE/SCC0611-MultHiper/Notas-simulado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Simulado</t>
   </si>
@@ -208,13 +208,16 @@
   </si>
   <si>
     <t>Identificação de Usuário</t>
+  </si>
+  <si>
+    <t>Sem Nome</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,13 +233,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -248,14 +263,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bom" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -576,7 +594,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
@@ -1274,6 +1292,14 @@
       </c>
       <c r="C62">
         <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" s="2">
+        <v>8.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>